<commit_message>
handling errors and time range options
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="PMC_Organoid_Japan" sheetId="1" r:id="rId1"/>
+    <sheet name="PMC_Organoid_Korea" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,23 +397,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" customWidth="1" width="182"/>
-    <col min="2" max="2" customWidth="1" width="21"/>
-    <col min="3" max="3" customWidth="1" width="24"/>
-    <col min="4" max="4" customWidth="1" width="39"/>
-    <col min="5" max="5" customWidth="1" width="205"/>
-    <col min="6" max="6" customWidth="1" width="27"/>
-    <col min="7" max="7" customWidth="1" width="45"/>
-    <col min="8" max="8" customWidth="1" width="205"/>
-    <col min="9" max="9" customWidth="1" width="27"/>
-    <col min="10" max="10" customWidth="1" width="35"/>
-    <col min="11" max="11" customWidth="1" width="192"/>
-    <col min="12" max="12" customWidth="1" width="55"/>
+    <col min="1" max="1" customWidth="1" width="164"/>
+    <col min="2" max="2" customWidth="1" width="17"/>
+    <col min="3" max="3" customWidth="1" width="23"/>
+    <col min="4" max="4" customWidth="1" width="24"/>
+    <col min="5" max="5" customWidth="1" width="257"/>
+    <col min="6" max="6" customWidth="1" width="21"/>
+    <col min="7" max="7" customWidth="1" width="33"/>
+    <col min="8" max="8" customWidth="1" width="257"/>
+    <col min="9" max="9" customWidth="1" width="23"/>
+    <col min="10" max="10" customWidth="1" width="27"/>
+    <col min="11" max="11" customWidth="1" width="257"/>
+    <col min="12" max="12" customWidth="1" width="50"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -456,1378 +456,1541 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Protocol to develop a proximal tubule-on-chip model based on hiPSC-derived kidney organoids for functional analysis of renal transporters</v>
+        <v>Recent Updates on Research Models and Tools to Study Virus–Host Interactions at the Placenta</v>
       </c>
       <c r="B2" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C2" t="str">
-        <v>Ma, Cheng</v>
-      </c>
-      <c r="D2" t="str">
-        <v>ma.cheng.5z@kyoto-u.ac.jp</v>
+        <v>Lee, Jae Kyung</v>
       </c>
       <c r="E2" t="str">
-        <v>Department of Micro Engineering, Kyoto University, Kyoto 615-8540, Japan</v>
+        <v>Department of Biomedical Sciences, College of Medicine, Korea University Guro Hospital, Seoul 08308 Korea;  (J.K.L.);  (S.-J.O.)</v>
       </c>
       <c r="F2" t="str">
-        <v>Yokokawa, Ryuji</v>
-      </c>
-      <c r="G2" t="str">
-        <v>yokokawa.ryuji.8c@kyoto-u.ac.jp</v>
+        <v>Shin, Ok Sarah</v>
       </c>
       <c r="H2" t="str">
-        <v>Department of Micro Engineering, Kyoto University, Kyoto 615-8540, Japan</v>
+        <v>Department of Biomedical Sciences, College of Medicine, Korea University Guro Hospital, Seoul 08308 Korea;  (J.K.L.);  (S.-J.O.)</v>
       </c>
       <c r="I2" t="str">
-        <v>Ma, Cheng</v>
-      </c>
-      <c r="J2" t="str">
-        <v>ma.cheng.5z@kyoto-u.ac.jp</v>
+        <v>Park, Hosun</v>
       </c>
       <c r="K2" t="str">
-        <v>Department of Micro Engineering, Kyoto University, Kyoto 615-8540, Japan</v>
+        <v>Department of Microbiology, College of Medicine, Yeungnam University, 170 Hyeonchung-ro, Namgu, Daegu 42415, Korea</v>
       </c>
       <c r="L2" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12225029/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC7020004/</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Causes and therapeutic limitations of clinical alopecia and the advent of human pluripotent stem cell follicular transplantation</v>
+        <v>LATS1 but not LATS2 represses autophagy by a kinase-independent scaffold function</v>
       </c>
       <c r="B3" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C3" t="str">
-        <v>Zhou, Hang</v>
+        <v>Tang, Fengyuan</v>
+      </c>
+      <c r="D3" t="str">
+        <v>fengyuan.tang@unibas.ch</v>
       </c>
       <c r="E3" t="str">
-        <v xml:space="preserve">Institute of Regenerative Medicine, Department of Dermatology, Affiliated Hospital of Jiangsu University, </v>
+        <v xml:space="preserve">Department of Biomedicine, University of Basel, </v>
       </c>
       <c r="F3" t="str">
-        <v>Zheng, Yun-Wen</v>
+        <v>Christofori, Gerhard</v>
       </c>
       <c r="G3" t="str">
-        <v>zhengyunwen@ihcams.ac.cn</v>
+        <v>gerhard.christofori@unibas.ch</v>
       </c>
       <c r="H3" t="str">
-        <v xml:space="preserve">Institute of Regenerative Medicine, Department of Dermatology, Affiliated Hospital of Jiangsu University, </v>
+        <v xml:space="preserve">Department of Biomedicine, University of Basel, </v>
       </c>
       <c r="L3" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12220152/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6917744/</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Liver developmental microenvironment promotes iHSC generation from human iPSCs</v>
+        <v>Kinase activity of ERBB3 contributes to intestinal organoids growth and intestinal tumorigenesis</v>
       </c>
       <c r="B4" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C4" t="str">
-        <v>Ye, Di</v>
+        <v>Nguyen, Anh Thai‐Quynh</v>
       </c>
       <c r="E4" t="str">
-        <v xml:space="preserve">Guangdong Provincial Key Laboratory of Large Animal Models for Biomedicine, and South China, Institute of Large Animal Models for Biomedicine, School of Pharmacy and FoodEngineering, Wuyi University, </v>
+        <v>cas14235-aff-0001</v>
       </c>
       <c r="F4" t="str">
-        <v>Zheng, Yun-Wen</v>
+        <v>Lee, Daekee</v>
       </c>
       <c r="G4" t="str">
-        <v>zhengyunwen@ihcams.ac.cn</v>
+        <v>daekee@ewha.ac.kr</v>
       </c>
       <c r="H4" t="str">
-        <v xml:space="preserve">Guangdong Provincial Key Laboratory of Large Animal Models for Biomedicine, and South China, Institute of Large Animal Models for Biomedicine, School of Pharmacy and FoodEngineering, Wuyi University, </v>
+        <v>cas14235-aff-0001</v>
       </c>
       <c r="L4" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12214545/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6942447/</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Narrative Review of Patient Cancer Tissue–Derived Zebrafish Xenograft Models for Evaluating Drug Sensitivity as an Avatar Model for Clinical Application</v>
+        <v>5-Fluorouracil as a Tumor-Treating Field-Sensitizer in Colon Cancer Therapy</v>
       </c>
       <c r="B5" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C5" t="str">
-        <v>Sugino, Yusuke</v>
+        <v>Lee, Yeon-Joo</v>
       </c>
       <c r="E5" t="str">
-        <v>cam470942-aff-0001</v>
+        <v>Division of Radiation Biomedical Research, Korea Institute of Radiological and Medical Sciences, Seoul 01812, Korea;  (Y.-J.L.);  (J.-M.C.);  (J.-Y.S.)</v>
       </c>
       <c r="F5" t="str">
-        <v>Inoue, Takahiro</v>
-      </c>
-      <c r="G5" t="str">
-        <v>tinoue28@med.mie-u.ac.jp</v>
+        <v>Kim, Eun Ho</v>
       </c>
       <c r="H5" t="str">
-        <v>cam470942-aff-0001</v>
+        <v xml:space="preserve">Department of Biochemistry, School of Medicine, Daegu Catholic University, 33, 17-gil, Duryugongwon-ro, Nam-gu, Daegu 42472, Korea; </v>
+      </c>
+      <c r="I5" t="str">
+        <v>Hwang, Sang-Gu</v>
+      </c>
+      <c r="K5" t="str">
+        <v>Division of Radiation Biomedical Research, Korea Institute of Radiological and Medical Sciences, Seoul 01812, Korea;  (Y.-J.L.);  (J.-M.C.);  (J.-Y.S.)</v>
       </c>
       <c r="L5" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12198658/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6966590/</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Regulation of disease signaling by YOD1: potential implications for therapeutic strategies</v>
+        <v>Neural Lineage Differentiation From Pluripotent Stem Cells to Mimic Human Brain Tissues</v>
       </c>
       <c r="B6" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C6" t="str">
-        <v>Zhao, Jiawei</v>
+        <v>Hong, Yean Ju</v>
       </c>
       <c r="E6" t="str">
-        <v xml:space="preserve">Key Laboratory of Tumor Immunology and Microenvironmental Regulation, Guilin Medical University, </v>
+        <v>Department of Stem Cell and Regenerative Biotechnology, KU Institute of Science and Technology, Konkuk University</v>
       </c>
       <c r="F6" t="str">
-        <v>Jin, Jiamin</v>
-      </c>
-      <c r="G6" t="str">
-        <v>jinjiamin@glmc.edu.cn</v>
+        <v>Do, Jeong Tae</v>
       </c>
       <c r="H6" t="str">
-        <v xml:space="preserve">Key Laboratory of Tumor Immunology and Microenvironmental Regulation, Guilin Medical University, </v>
+        <v>Department of Stem Cell and Regenerative Biotechnology, KU Institute of Science and Technology, Konkuk University</v>
+      </c>
+      <c r="I6" t="str">
+        <v>Do, Jeong Tae</v>
+      </c>
+      <c r="K6" t="str">
+        <v>Department of Stem Cell and Regenerative Biotechnology, KU Institute of Science and Technology, Konkuk University</v>
       </c>
       <c r="L6" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12188669/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6908493/</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Optimizing GBM organoid construction with hydrogel-based models: GelMA-HAMA scaffold supports GBM organoids with clonal growth for drug screening</v>
+        <v>Implication of  in colitis and homeostasis of intestinal epithelium</v>
       </c>
       <c r="B7" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C7" t="str">
-        <v>Zhou, Min</v>
+        <v>Seo, Yoojin</v>
       </c>
       <c r="E7" t="str">
-        <v>Shanghai Baoshan Luodian Hospital, School of Medicine, Shanghai University, Shanghai, China</v>
+        <v xml:space="preserve">Department of Life Science in Dentistry, School of Dentistry, Pusan National University, </v>
       </c>
       <c r="F7" t="str">
-        <v>Guo, Jianrong</v>
+        <v>Kim, Hyung-Sik</v>
+      </c>
+      <c r="G7" t="str">
+        <v>hskimcell@pusan.ac.kr</v>
       </c>
       <c r="H7" t="str">
-        <v>Department of Anesthesiology, Shanghai Pudong New Area Gongli Hospital, Shanghai, China</v>
-      </c>
-      <c r="I7" t="str">
-        <v>Guo, Jianrong</v>
-      </c>
-      <c r="K7" t="str">
-        <v>Department of Anesthesiology, Shanghai Pudong New Area Gongli Hospital, Shanghai, China</v>
+        <v xml:space="preserve">Department of Life Science in Dentistry, School of Dentistry, Pusan National University, </v>
       </c>
       <c r="L7" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12188089/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC7081540/</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Direct reprogramming of mouse fibroblasts into self-renewable alveolar epithelial-like cells</v>
+        <v>Graft immaturity and safety concerns in transplanted human kidney organoids</v>
       </c>
       <c r="B8" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C8" t="str">
-        <v>Morita, Atsuho</v>
+        <v>Nam, Sun Ah</v>
       </c>
       <c r="E8" t="str">
-        <v xml:space="preserve">Division of Pulmonary Medicine, Department of Medicine, Keio University School of Medicine, </v>
+        <v xml:space="preserve">Cell Death Disease Research Center, College of Medicine, The Catholic University of Korea, </v>
       </c>
       <c r="F8" t="str">
-        <v>Fukunaga, Koichi</v>
+        <v>Kim, Yong Kyun</v>
+      </c>
+      <c r="G8" t="str">
+        <v>drkimyk@catholic.ac.kr</v>
       </c>
       <c r="H8" t="str">
-        <v xml:space="preserve">Division of Pulmonary Medicine, Department of Medicine, Keio University School of Medicine, </v>
+        <v xml:space="preserve">Cell Death Disease Research Center, College of Medicine, The Catholic University of Korea, </v>
       </c>
       <c r="L8" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12185750/</v>
-      </c>
-    </row>
-    <row r="9" xml:space="preserve">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6881327/</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="str">
-        <v>How is the human microbiome linked to kidney stones?</v>
+        <v>Effective reconstruction of functional organotypic kidney spheroid for  nephrotoxicity studies</v>
       </c>
       <c r="B9" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C9" t="str">
-        <v>Pei, Xin</v>
-      </c>
-      <c r="E9" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-, , 
-</v>
+        <v>Kang, Hyun Mi</v>
+      </c>
+      <c r="E9" t="str">
+        <v xml:space="preserve">Laboratory of Disease Modeling and Therapeutics, Korea Research Institute of Bioscience and Biotechnology, </v>
       </c>
       <c r="F9" t="str">
-        <v>Yu, Shanshan</v>
-      </c>
-      <c r="H9" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-, , 
-</v>
+        <v>Jung, Cho-Rok</v>
+      </c>
+      <c r="G9" t="str">
+        <v>crjung@kribb.re.kr</v>
+      </c>
+      <c r="H9" t="str">
+        <v xml:space="preserve">Laboratory of Disease Modeling and Therapeutics, Korea Research Institute of Bioscience and Biotechnology, </v>
       </c>
       <c r="L9" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12179106/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6879515/</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Deep crypt secretory cells shape region-specific mucin glycosylation patterns in the mouse colon</v>
+        <v>Acetylation changes tau interactome to degrade tau in Alzheimer’s disease animal and organoid models</v>
       </c>
       <c r="B10" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C10" t="str">
-        <v>Sugahara, Daisuke</v>
+        <v>Choi, Heesun</v>
       </c>
       <c r="E10" t="str">
-        <v>aff001</v>
+        <v>acel13081-aff-0001</v>
       </c>
       <c r="F10" t="str">
-        <v>Akimoto, Yoshihiro</v>
+        <v>Mook‐Jung, Inhee</v>
+      </c>
+      <c r="G10" t="str">
+        <v>inhee@snu.ac.kr</v>
       </c>
       <c r="H10" t="str">
-        <v>aff001</v>
-      </c>
-      <c r="I10" t="str">
-        <v>Sugahara, Daisuke</v>
-      </c>
-      <c r="K10" t="str">
-        <v>aff001</v>
+        <v>acel13081-aff-0001</v>
       </c>
       <c r="L10" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12237016/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6974726/</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Transplantation of vascularized cardiac microtissue from human induced pluripotent stem cells improves impaired electrical conduction in a porcine myocardial injury model</v>
+        <v>Loss of Mob1a/b impairs the differentiation of mouse embryonic stem cells into the three germ layer lineages</v>
       </c>
       <c r="B11" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C11" t="str">
-        <v>Kuroda, Yuki</v>
+        <v>Bae, June Sung</v>
       </c>
       <c r="E11" t="str">
-        <v>Department of Cardiovascular Surgery, Graduate School of Medicine, Kyoto University, Kyoto, Japan</v>
+        <v xml:space="preserve">Research Institute, National Cancer Center, </v>
       </c>
       <c r="F11" t="str">
-        <v>Masumoto, Hidetoshi</v>
+        <v>Lee, Ho</v>
       </c>
       <c r="G11" t="str">
-        <v>masumoto@kuhp.kyoto-u.ac.jp</v>
+        <v>ho25lee@ncc.re.kr</v>
       </c>
       <c r="H11" t="str">
-        <v>Department of Cardiovascular Surgery, Graduate School of Medicine, Kyoto University, Kyoto, Japan</v>
-      </c>
-      <c r="I11" t="str">
-        <v>Masumoto, Hidetoshi</v>
-      </c>
-      <c r="J11" t="str">
-        <v>masumoto@kuhp.kyoto-u.ac.jp</v>
-      </c>
-      <c r="K11" t="str">
-        <v>Department of Cardiovascular Surgery, Graduate School of Medicine, Kyoto University, Kyoto, Japan</v>
+        <v xml:space="preserve">Research Institute, National Cancer Center, </v>
       </c>
       <c r="L11" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12230479/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6853965/</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Pancreatic cancer organoids derived from EUS-guided fine needle aspiration specimens can be used to predict chemotherapy resistance</v>
+        <v>Impact of mouse contamination in genomic profiling of patient-derived models and best practice for robust analysis</v>
       </c>
       <c r="B12" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C12" t="str">
-        <v>Oyama, Soshi</v>
+        <v>Jo, Se-Young</v>
       </c>
       <c r="E12" t="str">
-        <v xml:space="preserve">Department of Gastroenterology, Faculty of Medicine, Yamagata University, </v>
+        <v xml:space="preserve">Department of Biomedical Systems Informatics and Brain Korea 21 PLUS Project for Medical Science, Yonsei University College of Medicine, </v>
       </c>
       <c r="F12" t="str">
-        <v>Ueno, Yoshiyuki</v>
+        <v>Kim, Sangwoo</v>
+      </c>
+      <c r="G12" t="str">
+        <v>swkim@yuhs.ac</v>
       </c>
       <c r="H12" t="str">
-        <v xml:space="preserve">Department of Gastroenterology, Faculty of Medicine, Yamagata University, </v>
+        <v xml:space="preserve">Department of Biomedical Systems Informatics and Brain Korea 21 PLUS Project for Medical Science, Yonsei University College of Medicine, </v>
       </c>
       <c r="L12" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12229655/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6844030/</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Comprehensive characterization of human alveolar epithelial cells cultured for 28 days at the air-liquid interface</v>
+        <v>Microfluidic three-dimensional cell culture of stem cells for high-throughput analysis</v>
       </c>
       <c r="B13" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C13" t="str">
-        <v>Tanabe, Ikuya</v>
+        <v>Kim, Jeong Ah</v>
       </c>
       <c r="E13" t="str">
-        <v xml:space="preserve">Scientific Product Assessment Center, R&amp;D Group, Japan Tobacco Inc., </v>
+        <v/>
       </c>
       <c r="F13" t="str">
-        <v>Ishikawa, Shinkichi</v>
-      </c>
-      <c r="G13" t="str">
-        <v>shinkichi.ishikawa@jt.com</v>
+        <v>Rhee, Won Jong</v>
       </c>
       <c r="H13" t="str">
-        <v xml:space="preserve">Scientific Product Assessment Center, R&amp;D Group, Japan Tobacco Inc., </v>
+        <v/>
       </c>
       <c r="L13" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12219739/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6828593/</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Comprehensive gene expression analysis of organoid-derived healthy human colonic epithelium and cancer cell line stimulated with live probiotic bacteria</v>
+        <v>Microbial Metabolites Determine Host Health and the Status of Some Diseases</v>
       </c>
       <c r="B14" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C14" t="str">
-        <v>Sen, Akira</v>
+        <v>Sittipo, Panida</v>
       </c>
       <c r="E14" t="str">
-        <v xml:space="preserve">The Laboratory for Mucosal Ecosystem Design, Institute for Molecular and Cellular Regulation, Gunma University, </v>
+        <v/>
       </c>
       <c r="F14" t="str">
-        <v>Sasaki, Nobuo</v>
-      </c>
-      <c r="G14" t="str">
-        <v>nosasaki@gunma-u.ac.jp</v>
+        <v>Lee, Yun Kyung</v>
       </c>
       <c r="H14" t="str">
-        <v xml:space="preserve">The Laboratory for Mucosal Ecosystem Design, Institute for Molecular and Cellular Regulation, Gunma University, </v>
+        <v/>
+      </c>
+      <c r="I14" t="str">
+        <v>Shim, Jae-won</v>
+      </c>
+      <c r="K14" t="str">
+        <v/>
       </c>
       <c r="L14" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12217921/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6862038/</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Generation of mature epicardium derived from human-induced pluripotent stem cells via inhibition of mTOR signaling</v>
+        <v>A Cancer Spheroid Array Chip for Selecting Effective Drug</v>
       </c>
       <c r="B15" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C15" t="str">
-        <v>Tian, Yu</v>
+        <v>Choi, Jae Won</v>
       </c>
       <c r="E15" t="str">
-        <v xml:space="preserve">Center for iPS Cell Research and Application, Kyoto University, </v>
+        <v xml:space="preserve">Department of Biomedical Engineering, Konyang University, Daejeon 35365, Korea; </v>
       </c>
       <c r="F15" t="str">
-        <v>Yoshida, Yoshinori</v>
-      </c>
-      <c r="G15" t="str">
-        <v>yoshinor@cira.kyoto-u.ac.jp</v>
+        <v>Lee, Dong Woo</v>
       </c>
       <c r="H15" t="str">
-        <v xml:space="preserve">Center for iPS Cell Research and Application, Kyoto University, </v>
+        <v xml:space="preserve">Department of Biomedical Engineering, Konyang University, Daejeon 35365, Korea; </v>
+      </c>
+      <c r="I15" t="str">
+        <v>Lee, Dong Woo</v>
+      </c>
+      <c r="K15" t="str">
+        <v xml:space="preserve">Department of Biomedical Engineering, Konyang University, Daejeon 35365, Korea; </v>
       </c>
       <c r="L15" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12216149/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6843395/</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Activation of intestinal endogenous retroviruses by alcohol exacerbates liver disease</v>
+        <v>Development of human brain organoids with functional vascular-like system</v>
       </c>
       <c r="B16" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C16" t="str">
-        <v>Cabré, Noemí</v>
-      </c>
-      <c r="D16" t="str">
-        <v>ncabrecasares@health.ucsd.edu</v>
+        <v>Cakir, Bilal</v>
       </c>
       <c r="E16" t="str">
-        <v>Department of Medicine, University of California, San Diego, La Jolla, California, USA.</v>
+        <v>Department of Genetics, Yale Stem Cell Center, Yale School of Medicine, New Haven, CT 06520, USA.</v>
       </c>
       <c r="F16" t="str">
-        <v>Schnabl, Bernd</v>
-      </c>
-      <c r="G16" t="str">
-        <v>beschnabl@ucsd.edu</v>
+        <v>Park, In-Hyun</v>
       </c>
       <c r="H16" t="str">
-        <v>Department of Medicine, University of California, San Diego, La Jolla, California, USA.</v>
+        <v>Department of Genetics, Yale Stem Cell Center, Yale School of Medicine, New Haven, CT 06520, USA.</v>
+      </c>
+      <c r="I16" t="str">
+        <v>Park, In-Hyun</v>
+      </c>
+      <c r="K16" t="str">
+        <v>Department of Genetics, Yale Stem Cell Center, Yale School of Medicine, New Haven, CT 06520, USA.</v>
       </c>
       <c r="L16" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12208555/</v>
-      </c>
-    </row>
-    <row r="17" xml:space="preserve">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6918722/</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" t="str">
-        <v>High-Throughput Drug Screening of Clear Cell Ovarian Cancer Organoids Reveals Vulnerability to Proteasome Inhibitors and Dinaciclib and Identifies AGR2 as a Therapeutic Target</v>
+        <v>RORα is crucial for attenuated inflammatory response to maintain intestinal homeostasis</v>
       </c>
       <c r="B17" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C17" t="str">
-        <v>Yoshimura, Takuma</v>
-      </c>
-      <c r="E17" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Department of Obstetrics and Gynecology, Keio University School of Medicine, Tokyo, Japan.</v>
+        <v>Oh, Se Kyu</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Creative Research Initiatives Center for Epigenetic Code and Diseases, School of Biological Sciences, , 08826 Seoul, ;</v>
       </c>
       <c r="F17" t="str">
-        <v>Chiyoda, Tatsuyuki</v>
-      </c>
-      <c r="H17" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Department of Obstetrics and Gynecology, Keio University School of Medicine, Tokyo, Japan.</v>
+        <v>Baek, Sung Hee</v>
+      </c>
+      <c r="H17" t="str">
+        <v>Creative Research Initiatives Center for Epigenetic Code and Diseases, School of Biological Sciences, , 08826 Seoul, ;</v>
       </c>
       <c r="I17" t="str">
-        <v>Tsunoda, Tatsuhiko</v>
-      </c>
-      <c r="K17" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Laboratory for Medical Science Mathematics, Department of Biological Sciences, School of Science, The University of Tokyo, Tokyo, Japan.</v>
+        <v>Park, Daechan</v>
+      </c>
+      <c r="K17" t="str">
+        <v xml:space="preserve">Department of Biological Sciences, College of Natural Sciences, , 16499 Suwon, </v>
       </c>
       <c r="L17" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12188421/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6800319/</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>In vitro generation of a ureteral organoid from pluripotent stem cells</v>
+        <v>Past, Present, and Future of Brain Organoid Technology</v>
       </c>
       <c r="B18" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C18" t="str">
-        <v>Ibi, Yutaro</v>
+        <v>Koo, Bonsang</v>
       </c>
       <c r="E18" t="str">
-        <v xml:space="preserve">Department of Kidney Development, Institute of Molecular Embryology and Genetics, Kumamoto University, </v>
+        <v/>
       </c>
       <c r="F18" t="str">
-        <v>Nishinakamura, Ryuichi</v>
-      </c>
-      <c r="G18" t="str">
-        <v>ryuichi@kumamoto-u.ac.jp</v>
+        <v>Yoon, Ki-Jun</v>
       </c>
       <c r="H18" t="str">
-        <v xml:space="preserve">Department of Kidney Development, Institute of Molecular Embryology and Genetics, Kumamoto University, </v>
+        <v/>
+      </c>
+      <c r="I18" t="str">
+        <v>Yoon, Ki-Jun</v>
+      </c>
+      <c r="K18" t="str">
+        <v/>
       </c>
       <c r="L18" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12181279/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6776157/</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Application of human iPSC-derived white, beige, and brown adipocytes for metabolic disease modeling and transplantation therapy</v>
+        <v>Development of Patient-Derived Preclinical Platform for Metastatic Pancreatic Cancer: PDOX and a Subsequent Organoid Model System Using Percutaneous Biopsy Samples</v>
       </c>
       <c r="B19" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C19" t="str">
-        <v>Keidai, Yamato</v>
+        <v>Choi, Sun Il</v>
       </c>
       <c r="E19" t="str">
-        <v>Department of Diabetes, Endocrinology and Nutrition, Graduate School of Medicine, Kyoto University, Kyoto, Japan</v>
+        <v xml:space="preserve">, , </v>
       </c>
       <c r="F19" t="str">
-        <v>Yabe, Daisuke</v>
+        <v>Kim, Yun-Hee</v>
       </c>
       <c r="H19" t="str">
-        <v>Department of Diabetes, Endocrinology and Nutrition, Graduate School of Medicine, Kyoto University, Kyoto, Japan</v>
+        <v xml:space="preserve">, , </v>
       </c>
       <c r="I19" t="str">
-        <v>Fujikura, Junji</v>
+        <v>Woo, Sang Myung</v>
       </c>
       <c r="K19" t="str">
-        <v>Department of Diabetes, Endocrinology and Nutrition, Graduate School of Medicine, Kyoto University, Kyoto, Japan</v>
+        <v xml:space="preserve">, , </v>
       </c>
       <c r="L19" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12179452/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6753223/</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Colorectal cancer cell line-derived organoid model with stem cell properties captures the regrowing state of residual cancer cells after neoadjuvant chemotherapy</v>
+        <v>Perturbed myoepithelial cell differentiation in  mutation carriers and in ductal carcinoma in situ</v>
       </c>
       <c r="B20" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C20" t="str">
-        <v>Nakano, Kiyotaka</v>
-      </c>
-      <c r="D20" t="str">
-        <v>nakanokyt@chugai-pharm.co.jp</v>
+        <v>Ding, Lina</v>
       </c>
       <c r="E20" t="str">
-        <v xml:space="preserve">Translational Research Division, Chugai Pharmaceutical Co., Ltd., Chugai Life Science Park Yokohama 216 Totsuka-cho, Totsuka-ku, </v>
+        <v xml:space="preserve">Department of Medical Oncology, Dana-Farber Cancer Institute Boston, </v>
       </c>
       <c r="F20" t="str">
-        <v>Yamazaki, Tatsumi</v>
+        <v>Polyak, Kornelia</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Kornelia_Polyak@dfci.harvard.edu</v>
       </c>
       <c r="H20" t="str">
-        <v xml:space="preserve">Central Institute for Experimental Medicine and Life Science, 3-25-12 Tonomachi, Kawasaki-ku, Kawasaki, 210-0821 Japan </v>
+        <v xml:space="preserve">Department of Medical Oncology, Dana-Farber Cancer Institute Boston, </v>
       </c>
       <c r="L20" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12179298/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6744561/</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>How chronic inflammation fuels carcinogenesis as an environmental epimutagen</v>
+        <v>Worm-Based Alternate Assessment of Probiotic Intervention against Gut Barrier Infection</v>
       </c>
       <c r="B21" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C21" t="str">
-        <v>Liu, Yu-Yu</v>
+        <v>Kim, Juil</v>
       </c>
       <c r="E21" t="str">
-        <v xml:space="preserve">Department of Epigenomics, Institute for Advanced Life Sciences, Hoshi University, </v>
+        <v>Laboratory of Mucosal Exposome and Biomodulation, Department of Biomedical Sciences and Biomedical Research Institute, Pusan National University, Yangsan 50612, Korea</v>
       </c>
       <c r="F21" t="str">
-        <v>Ushijima, Toshikazu</v>
-      </c>
-      <c r="G21" t="str">
-        <v>tushijima142@hoshi.ac.jp</v>
+        <v>Moon, Yuseok</v>
       </c>
       <c r="H21" t="str">
-        <v xml:space="preserve">Department of Epigenomics, Institute for Advanced Life Sciences, Hoshi University, </v>
+        <v>Laboratory of Mucosal Exposome and Biomodulation, Department of Biomedical Sciences and Biomedical Research Institute, Pusan National University, Yangsan 50612, Korea</v>
+      </c>
+      <c r="I21" t="str">
+        <v>Moon, Yuseok</v>
+      </c>
+      <c r="K21" t="str">
+        <v>Laboratory of Mucosal Exposome and Biomodulation, Department of Biomedical Sciences and Biomedical Research Institute, Pusan National University, Yangsan 50612, Korea</v>
       </c>
       <c r="L21" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12176710/</v>
-      </c>
-    </row>
-    <row r="22" xml:space="preserve">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6770392/</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" t="str">
-        <v>An Acrolein-Based Drug Delivery System Enables Tumor-Specific Sphingosine-1-Phosphate Targeting in Breast Cancer without Lymphocytopenia</v>
+        <v>Summit proceedings: Biomedical countermeasure development for emerging vector-borne viral diseases</v>
       </c>
       <c r="B22" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C22" t="str">
-        <v>Nagahashi, Masayuki</v>
-      </c>
-      <c r="E22" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Division of Breast and Endocrine Surgery, Department of Surgery, Hyogo Medical University, Nishinomiya, Japan.</v>
+        <v>Blackman, Marcia A.</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Trudeau Institute, Saranac Lake, NY, USA</v>
       </c>
       <c r="F22" t="str">
-        <v>Miyoshi, Yasuo</v>
-      </c>
-      <c r="H22" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Division of Breast and Endocrine Surgery, Department of Surgery, Hyogo Medical University, Nishinomiya, Japan.</v>
+        <v>Thomas, Stephen J.</v>
+      </c>
+      <c r="H22" t="str">
+        <v>Division of Infectious Diseases, State University of New York, Upstate Medical University, Syracuse, NY, USA</v>
       </c>
       <c r="I22" t="str">
-        <v>Nagahashi, Masayuki</v>
-      </c>
-      <c r="K22" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Division of Breast and Endocrine Surgery, Department of Surgery, Hyogo Medical University, Nishinomiya, Japan.</v>
+        <v>Thomas, Stephen J.</v>
+      </c>
+      <c r="K22" t="str">
+        <v>Division of Infectious Diseases, State University of New York, Upstate Medical University, Syracuse, NY, USA</v>
       </c>
       <c r="L22" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12174973/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC7131820/</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Axillary adipose tissue–derived lymphatic endothelial cells exhibit distinct transcriptomic signatures reflecting lymphatic invasion status in breast cancer</v>
+        <v>Patient-derived lung cancer organoids as in vitro cancer models for therapeutic screening</v>
       </c>
       <c r="B23" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C23" t="str">
-        <v>Iesato, Asumi</v>
+        <v>Kim, Minsuh</v>
       </c>
       <c r="E23" t="str">
-        <v xml:space="preserve">NEXT-Ganken Program, Cancer Cell Diversity Project, Japanese Foundation for Cancer Research, </v>
+        <v xml:space="preserve">Asan Center for Cancer Genome Discovery, Asan Institute for Life Sciences, </v>
       </c>
       <c r="F23" t="str">
-        <v>Maruyama, Reo</v>
+        <v>Jang, Se Jin</v>
       </c>
       <c r="G23" t="str">
-        <v>reo.maruyama@jfcr.or.jp</v>
+        <v>jangsejin@amc.seoul.kr</v>
       </c>
       <c r="H23" t="str">
-        <v xml:space="preserve">NEXT-Ganken Program, Cancer Cell Diversity Project, Japanese Foundation for Cancer Research, </v>
+        <v xml:space="preserve">Asan Center for Cancer Genome Discovery, Asan Institute for Life Sciences, </v>
       </c>
       <c r="L23" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12172209/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6728380/</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Evaluation of Organoid‐Derived Exosomal  as Liquid Biopsy for Colorectal Cancer: A Multicenter Cross‐Sectional Study</v>
+        <v>NOD2 Supports Crypt Survival and Epithelial Regeneration after Radiation-Induced Injury</v>
       </c>
       <c r="B24" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C24" t="str">
-        <v>Sasaki, Atsuhiro</v>
+        <v>Lee, Chansu</v>
       </c>
       <c r="E24" t="str">
-        <v>cts70270-aff-0001</v>
+        <v>Department of Medicine, Samsung Medical Center, Sungkyunwan University School of Medicine, Seoul 06351, Korea</v>
       </c>
       <c r="F24" t="str">
-        <v>Masamune, Atsushi</v>
+        <v>Hong, Sung Noh</v>
       </c>
       <c r="H24" t="str">
-        <v>cts70270-aff-0001</v>
+        <v>Department of Medicine, Samsung Medical Center, Sungkyunwan University School of Medicine, Seoul 06351, Korea</v>
+      </c>
+      <c r="I24" t="str">
+        <v>Park, Hee Chul</v>
+      </c>
+      <c r="K24" t="str">
+        <v>Department of Radiation Oncology, Samsung Medical Center, Seoul 06351, Korea</v>
       </c>
       <c r="L24" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12166945/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6747113/</v>
       </c>
     </row>
     <row r="25" xml:space="preserve">
       <c r="A25" t="str">
-        <v>Dual Role of NRF2 in Pancreatic Precursor Lesions</v>
+        <v>Baicalein Mitigates Radiation-Induced Enteritis by Improving Endothelial Dysfunction</v>
       </c>
       <c r="B25" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C25" t="str">
-        <v>Ichimiya, Shu</v>
+        <v>Jang, Hyosun</v>
       </c>
       <c r="E25" t="str" xml:space="preserve">
         <v xml:space="preserve">
-Department of Genetics and Development, Institute for Cancer Genetics, Columbia University Irving Medical Center, New York, New York.</v>
+, , </v>
       </c>
       <c r="F25" t="str">
-        <v>Chio, Iok In Christine</v>
+        <v>Myung, Jae kyung</v>
       </c>
       <c r="H25" t="str" xml:space="preserve">
         <v xml:space="preserve">
-Department of Genetics and Development, Institute for Cancer Genetics, Columbia University Irving Medical Center, New York, New York.</v>
-      </c>
-      <c r="I25" t="str">
-        <v>Chio, Iok In Christine</v>
-      </c>
-      <c r="K25" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Department of Genetics and Development, Institute for Cancer Genetics, Columbia University Irving Medical Center, New York, New York.</v>
+, , </v>
       </c>
       <c r="L25" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12158068/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6707809/</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Primitive Hepatoblasts Driving Early Liver Development</v>
+        <v>Intestinal enteroids/organoids: A novel platform for drug discovery in inflammatory bowel diseases</v>
       </c>
       <c r="B26" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C26" t="str">
-        <v>Iwasawa, Kentaro</v>
+        <v>Yoo, Jun-Hwan</v>
       </c>
       <c r="E26" t="str">
-        <v>Division of Gastroenterology, Hepatology &amp; Nutrition, Cincinnati Children’s Hospital Medical Center, 3333 Burnet Avenue, Cincinnati, OH 45229-3039, USA</v>
+        <v/>
       </c>
       <c r="F26" t="str">
-        <v>Takebe, Takanori</v>
+        <v>Donowitz, Mark</v>
       </c>
       <c r="H26" t="str">
-        <v>Division of Gastroenterology, Hepatology &amp; Nutrition, Cincinnati Children’s Hospital Medical Center, 3333 Burnet Avenue, Cincinnati, OH 45229-3039, USA</v>
+        <v/>
       </c>
       <c r="L26" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12157602/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6700704/</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Single-cell transcriptome sequencing reveals new epithelial-stromal associated mesenchymal-like subsets in recurrent gliomas</v>
+        <v>Clinical Implementation of Precision Medicine in Gastric Cancer</v>
       </c>
       <c r="B27" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C27" t="str">
-        <v>Li, Jinwei</v>
+        <v>Jeon, Jaewook</v>
       </c>
       <c r="E27" t="str">
-        <v xml:space="preserve">Department of Neurosurgery, Beijing Tiantan Hospital, Capital Medical University, </v>
+        <v>Yonsei University College of Medicine, Seoul, .</v>
       </c>
       <c r="F27" t="str">
-        <v>Wang, Yinyan</v>
-      </c>
-      <c r="G27" t="str">
-        <v>tiantanyinyan@126.com</v>
+        <v>Cheong, Jae-Ho</v>
       </c>
       <c r="H27" t="str">
-        <v xml:space="preserve">Department of Neurosurgery, Beijing Tiantan Hospital, Capital Medical University, </v>
+        <v>Department of Surgery, Yonsei University College of Medicine, Seoul, .</v>
       </c>
       <c r="L27" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12145596/</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6769368/</v>
+      </c>
+    </row>
+    <row r="28" xml:space="preserve">
       <c r="A28" t="str">
-        <v>Heterochronic pelvic high-grade myxoinflammatory fibroblastic sarcoma and uterine endometroid carcinoma harboring common gene mutations: a rare case report with genomic analysis</v>
+        <v>Human Induced Pluripotent Stem Cells : Clinical Significance and Applications in Neurologic Diseases</v>
       </c>
       <c r="B28" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C28" t="str">
-        <v>Higashi, Yuriko</v>
-      </c>
-      <c r="E28" t="str">
-        <v xml:space="preserve">Department of Pathology, Kagoshima University Graduate School of Medical and Dental Sciences, </v>
+        <v>Chang, Eun-Ah</v>
+      </c>
+      <c r="E28" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Laboratory Medicine, Korea University Ansan Hospital, Ansan, </v>
       </c>
       <c r="F28" t="str">
-        <v>Tanimoto, Akihide</v>
-      </c>
-      <c r="G28" t="str">
-        <v>akit09@m3.kufm.kagoshima-u.ac.jp</v>
-      </c>
-      <c r="H28" t="str">
-        <v xml:space="preserve">Department of Pathology, Kagoshima University Graduate School of Medical and Dental Sciences, </v>
+        <v>Kim, Sang-Dae</v>
+      </c>
+      <c r="H28" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Neurosurgery, Korea University Ansan Hospital, Ansan, </v>
+      </c>
+      <c r="I28" t="str">
+        <v>Kim, Sang-Dae</v>
+      </c>
+      <c r="K28" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Neurosurgery, Korea University Ansan Hospital, Ansan, </v>
       </c>
       <c r="L28" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12131376/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6732359/</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Stepwise strategy for generating human trophoblast stem-like cells from embryonic stem cells reveals specific role of TFAP2C in acquiring self-renewability</v>
+        <v>Targeting CYP4A attenuates hepatic steatosis in a novel multicellular organotypic liver model</v>
       </c>
       <c r="B29" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C29" t="str">
-        <v>Ohgushi, Masatoshi</v>
-      </c>
-      <c r="D29" t="str">
-        <v>ohgushi.masatoshi.5r@kyoto-u.ac.jp</v>
+        <v>Ryu, Jae-Sung</v>
       </c>
       <c r="E29" t="str">
-        <v xml:space="preserve">Laboratory of Developmental Systems, Institute for Life and Medical Sciences, Kyoto University, </v>
+        <v xml:space="preserve">Stem Cell Convergence Research Center, Korea Research Institute of Bioscience and Biotechnology (KRIBB), </v>
       </c>
       <c r="F29" t="str">
-        <v>Eiraku, Mototsugu</v>
+        <v>Son, Myung Jin</v>
+      </c>
+      <c r="G29" t="str">
+        <v>mjson@kribb.re.kr</v>
       </c>
       <c r="H29" t="str">
-        <v xml:space="preserve">Laboratory of Developmental Systems, Institute for Life and Medical Sciences, Kyoto University, </v>
+        <v xml:space="preserve">Stem Cell Convergence Research Center, Korea Research Institute of Bioscience and Biotechnology (KRIBB), </v>
       </c>
       <c r="L29" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12125314/</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6686528/</v>
+      </c>
+    </row>
+    <row r="30" xml:space="preserve">
       <c r="A30" t="str">
-        <v>Current status, hotspots, and trends in cancer prevention, screening, diagnosis, treatment, and rehabilitation: A bibliometric analysis</v>
+        <v>Pancreatic High-Grade Neuroendocrine Neoplasms in the Korean Population: A Multicenter Study</v>
       </c>
       <c r="B30" t="str">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C30" t="str">
-        <v>ZHANG, CHUCHU</v>
-      </c>
-      <c r="E30" t="str">
-        <v xml:space="preserve">, , </v>
+        <v>Kim, Haeryoung</v>
+      </c>
+      <c r="E30" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Pathology, Seoul National University Hospital, Seoul, </v>
       </c>
       <c r="F30" t="str">
-        <v>LI, HAIYAN</v>
-      </c>
-      <c r="G30" t="str">
-        <v>li_haiyan01@126.com</v>
-      </c>
-      <c r="H30" t="str">
-        <v xml:space="preserve">, , </v>
+        <v>Hong, Seung-Mo</v>
+      </c>
+      <c r="H30" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Pathology, Asan Medical Center, University of Ulsan College of Medicine, Seoul, </v>
+      </c>
+      <c r="I30" t="str">
+        <v>Kim, Youn Wha</v>
+      </c>
+      <c r="K30" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Pathology, Kyung Hee University College of Medicine, Seoul, </v>
       </c>
       <c r="L30" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12144630/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6962471/</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>From bench to bedside: the role of gastrointestinal stem cells in health and disease</v>
+        <v>Targeting Cancer Stem Cells in Triple-Negative Breast Cancer</v>
       </c>
       <c r="B31" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C31" t="str">
-        <v>Bai, Xiaopeng</v>
+        <v>Park, So-Yeon</v>
       </c>
       <c r="E31" t="str">
-        <v xml:space="preserve">Department of Medicine and Bioregulatory Science, Graduate School of Medical Sciences, Kyushu University, </v>
+        <v>School of Life Sciences, Gwangju Institute of Science and Technology, Gwangju 61005, Korea</v>
       </c>
       <c r="F31" t="str">
-        <v>Ogawa, Yoshihiro</v>
+        <v>Nam, Jeong-Seok</v>
       </c>
       <c r="H31" t="str">
-        <v xml:space="preserve">Department of Medicine and Bioregulatory Science, Graduate School of Medical Sciences, Kyushu University, </v>
+        <v>School of Life Sciences, Gwangju Institute of Science and Technology, Gwangju 61005, Korea</v>
+      </c>
+      <c r="I31" t="str">
+        <v>Nam, Jeong-Seok</v>
+      </c>
+      <c r="K31" t="str">
+        <v>School of Life Sciences, Gwangju Institute of Science and Technology, Gwangju 61005, Korea</v>
       </c>
       <c r="L31" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12117945/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6678244/</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>In Silico Identification and Characterization of Spiro[1,2,4]triazolo[1,5-]quinazolines as Diacylglycerol Kinase α Modulators</v>
+        <v>Antioxidant therapy in chronic pancreatitis—promises and pitfalls</v>
       </c>
       <c r="B32" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C32" t="str">
-        <v>Antypenko, Lyudmyla</v>
+        <v>Ko, Kwang Hyun</v>
       </c>
       <c r="E32" t="str">
-        <v>Independent Researcher, 11 Lamana Str., 69063 Zaporizhzhia, Ukraine</v>
+        <v>Digestive Disease Center, CHA University Bundang Medical Center, Seongnam, ;</v>
       </c>
       <c r="F32" t="str">
-        <v>Kovalenko, Serhii</v>
+        <v>Hahm, Ki Baik</v>
       </c>
       <c r="H32" t="str">
-        <v xml:space="preserve">Institute of Chemistry and Geology, Oles Honchar Dnipro National University, 72 Nauky Ave., 49010 Dnipro, Ukraine; </v>
-      </c>
-      <c r="I32" t="str">
-        <v>Antypenko, Lyudmyla</v>
-      </c>
-      <c r="K32" t="str">
-        <v>Independent Researcher, 11 Lamana Str., 69063 Zaporizhzhia, Ukraine</v>
+        <v>Digestive Disease Center, CHA University Bundang Medical Center, Seongnam, ;</v>
       </c>
       <c r="L32" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12156019/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6685855/</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Shaking culture attenuates circadian rhythms in induced pluripotent stem cells during osteogenic differentiation through the TEAD-Fbxl3-CRY axis</v>
+        <v>KRAS activation in gastric adenocarcinoma stimulates epithelial-to-mesenchymal transition to cancer stem-like cells and promotes metastasis</v>
       </c>
       <c r="B33" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C33" t="str">
-        <v>Fu, Yunyu</v>
+        <v>Yoon, Changhwan</v>
       </c>
       <c r="E33" t="str">
-        <v xml:space="preserve">Division of Molecular and Regenerative Prosthodontics, Tohoku University Graduate School of Dentistry, </v>
+        <v>Gastric and Mixed Tumor Service, Department of Surgery, Memorial Sloan Kettering Cancer Center, New York, NY</v>
       </c>
       <c r="F33" t="str">
-        <v>Egusa, Hiroshi</v>
-      </c>
-      <c r="G33" t="str">
-        <v>egu@tohoku.ac.jp</v>
+        <v>Yoon, Sam S.</v>
       </c>
       <c r="H33" t="str">
-        <v xml:space="preserve">Division of Molecular and Regenerative Prosthodontics, Tohoku University Graduate School of Dentistry, </v>
+        <v>Gastric and Mixed Tumor Service, Department of Surgery, Memorial Sloan Kettering Cancer Center, New York, NY</v>
       </c>
       <c r="L33" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12103599/</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6726517/</v>
+      </c>
+    </row>
+    <row r="34" xml:space="preserve">
       <c r="A34" t="str">
-        <v>Induced Pluripotent Stem Cells in Cardiomyopathy: Advancing Disease Modeling, Therapeutic Development, and Regenerative Therapy</v>
+        <v>Development of Collagen-Based 3D Matrix for Gastrointestinal Tract-Derived Organoid Culture</v>
       </c>
       <c r="B34" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C34" t="str">
-        <v>Vo, Quan Duy</v>
-      </c>
-      <c r="E34" t="str">
-        <v>Department of Cardiovascular Medicine, Okayama University Graduate School of Medicine, Dentistry and Pharmaceutical Sciences, Okayama 700-8558, Japan;  (Q.D.V.);  (S.A.);  (T.M.);  (S.Y.)</v>
+        <v>Jee, Joo Hyun</v>
+      </c>
+      <c r="E34" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Microbiology, School of Medicine, CHA University, Seongnam-si, Gyeonggi-do 13488, Republic of Korea</v>
       </c>
       <c r="F34" t="str">
-        <v>Yuasa, Shinsuke</v>
-      </c>
-      <c r="H34" t="str">
-        <v>Department of Cardiovascular Medicine, Okayama University Graduate School of Medicine, Dentistry and Pharmaceutical Sciences, Okayama 700-8558, Japan;  (Q.D.V.);  (S.A.);  (T.M.);  (S.Y.)</v>
-      </c>
-      <c r="I34" t="str">
-        <v>Nakamura, Kazufumi</v>
-      </c>
-      <c r="K34" t="str">
-        <v>Department of Cardiovascular Medicine, Okayama University Graduate School of Medicine, Dentistry and Pharmaceutical Sciences, Okayama 700-8558, Japan;  (Q.D.V.);  (S.A.);  (T.M.);  (S.Y.)</v>
+        <v>Yoo, Jongman</v>
+      </c>
+      <c r="G34" t="str">
+        <v>jongmanyoo@cha.ac.kr</v>
+      </c>
+      <c r="H34" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Microbiology, School of Medicine, CHA University, Seongnam-si, Gyeonggi-do 13488, Republic of Korea</v>
       </c>
       <c r="L34" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12155407/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6595382/</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>CDX1 and CDX2 suppress colon cancer stemness by inhibiting β-catenin-facilitated formation of Pol II–DSIF–PAF1C complex</v>
+        <v>Recent advances in organoid culture for insulin production and diabetes therapy: methods and challenges</v>
       </c>
       <c r="B35" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C35" t="str">
-        <v>Aoki, Koji</v>
-      </c>
-      <c r="D35" t="str">
-        <v>aokik@u-fukui.ac.jp</v>
+        <v>Dayem, Ahmed Abdal</v>
       </c>
       <c r="E35" t="str">
-        <v xml:space="preserve">Department of Pharmacology, Faculty of Medicine, University of Fukui, </v>
+        <v/>
       </c>
       <c r="F35" t="str">
-        <v>Igarashi, Ayumi</v>
+        <v>Cho, Ssang-Goo</v>
       </c>
       <c r="H35" t="str">
-        <v xml:space="preserve">Department of Pharmacology, Faculty of Medicine, University of Fukui, </v>
+        <v/>
+      </c>
+      <c r="I35" t="str">
+        <v>Cho, Ssang-Goo</v>
+      </c>
+      <c r="K35" t="str">
+        <v/>
       </c>
       <c r="L35" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12095478/</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6549913/</v>
+      </c>
+    </row>
+    <row r="36" xml:space="preserve">
       <c r="A36" t="str">
-        <v>Cardiac organoids: a new tool for disease modeling and drug screening applications</v>
+        <v>Transplantation of Mature Photoreceptors in Rodents With Retinal Degeneration</v>
       </c>
       <c r="B36" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C36" t="str">
-        <v>Yaqinuddin, Ahmed</v>
-      </c>
-      <c r="E36" t="str">
-        <v xml:space="preserve">, , </v>
+        <v>Lorach, Henri</v>
+      </c>
+      <c r="E36" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Hansen Experimental Physics Laboratory, Stanford University, CA, USA
+</v>
       </c>
       <c r="F36" t="str">
-        <v>Mir, Tanveer Ahmad</v>
-      </c>
-      <c r="H36" t="str">
-        <v xml:space="preserve">, , </v>
-      </c>
-      <c r="I36" t="str">
-        <v>Yaqinuddin, Ahmed</v>
-      </c>
-      <c r="K36" t="str">
-        <v xml:space="preserve">, , </v>
+        <v>Palanker, Daniel</v>
+      </c>
+      <c r="H36" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Hansen Experimental Physics Laboratory, Stanford University, CA, USA
+</v>
       </c>
       <c r="L36" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12129933/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6543858/</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Preface of the special issue “Mechanisms of reprogramming for cell differentiation and tissue regeneration”</v>
+        <v>Which Needle Needs to Be Chosen for Better Outcome of Endoscopic Ultrasound-Guided Tissue Acquisition?</v>
       </c>
       <c r="B37" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C37" t="str">
-        <v>Shiota, Goshi</v>
-      </c>
-      <c r="D37" t="str">
-        <v>gshiota@tottori-u.ac.jp</v>
+        <v>Lee, Dong Wook</v>
       </c>
       <c r="E37" t="str">
         <v/>
       </c>
       <c r="F37" t="str">
-        <v>Shiota, Goshi</v>
-      </c>
-      <c r="G37" t="str">
-        <v>gshiota@tottori-u.ac.jp</v>
+        <v>Kim, Eun Young</v>
       </c>
       <c r="H37" t="str">
         <v/>
       </c>
       <c r="L37" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12146485/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6529168/</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Establishment of an  implantation model using a newly developed mouse endometrial organoid</v>
+        <v>Receptor subtype discrimination using extensive shape complementary designed interfaces</v>
       </c>
       <c r="B38" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C38" t="str">
-        <v>Fujimura, Taishi</v>
+        <v>Dang, Luke T.</v>
       </c>
       <c r="E38" t="str">
-        <v xml:space="preserve">, , , </v>
+        <v>Department of Biochemistry, University of Washington, Seattle, Washington 98105, USA</v>
       </c>
       <c r="F38" t="str">
-        <v>Sugino, Norihiro</v>
+        <v>Baker, David</v>
       </c>
       <c r="H38" t="str">
-        <v xml:space="preserve">, , , </v>
+        <v>Department of Biochemistry, University of Washington, Seattle, Washington 98105, USA</v>
       </c>
       <c r="I38" t="str">
-        <v>Tamura, Isao</v>
-      </c>
-      <c r="J38" t="str">
-        <v>isao@yamaguchi-u.ac.jp</v>
+        <v>Garcia, K. Christopher</v>
       </c>
       <c r="K38" t="str">
-        <v xml:space="preserve">, , , </v>
+        <v>Department of Molecular and Cellular Physiology, Stanford University School of Medicine, Stanford, California 94305, USA</v>
       </c>
       <c r="L38" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12091871/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6582999/</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>LCN2-mediated ferroptosis resistance in tissue homeostasis and early-stage tumorigenesis of the fallopian tube epithelium</v>
+        <v>Human 3D Cellular Model of Hypoxic Brain Injury of Prematurity</v>
       </c>
       <c r="B39" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C39" t="str">
-        <v>Imaeda, Keiyo</v>
+        <v>Paşca, Anca M.</v>
       </c>
       <c r="E39" t="str">
-        <v>Department of Obstetrics and Gynecology, Keio University School of Medicine, Tokyo, Japan</v>
+        <v>Department of Pediatrics, Division of Neonatology, Stanford University School of Medicine, Stanford, CA 94305, USA</v>
       </c>
       <c r="F39" t="str">
-        <v>Yamagami, Wataru</v>
+        <v>Paşca, Sergiu P.</v>
       </c>
       <c r="H39" t="str">
-        <v>Department of Obstetrics and Gynecology, Keio University School of Medicine, Tokyo, Japan</v>
+        <v>Department of Psychiatry and Behavioral Sciences, Stanford University School of Medicine, Stanford, CA 94305, USA</v>
       </c>
       <c r="I39" t="str">
-        <v>Masuda, Kenta</v>
-      </c>
-      <c r="J39" t="str">
-        <v>ma-su-ken.a2@keio.jp</v>
+        <v>Paşca, Sergiu P.</v>
       </c>
       <c r="K39" t="str">
-        <v>Department of Obstetrics and Gynecology, Keio University School of Medicine, Tokyo, Japan</v>
+        <v>Department of Psychiatry and Behavioral Sciences, Stanford University School of Medicine, Stanford, CA 94305, USA</v>
       </c>
       <c r="L39" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12158494/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC7020938/</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Basal-shift transformation leads to EGFR therapy-resistance in human lung adenocarcinoma</v>
+        <v>Association of pathway mutation with survival after recurrence in colorectal cancer patients treated with adjuvant fluoropyrimidine and oxaliplatin chemotherapy</v>
       </c>
       <c r="B40" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C40" t="str">
-        <v>Shinozaki, Taro</v>
+        <v>Lee, Dae-Won</v>
+      </c>
+      <c r="D40" t="str">
+        <v>silver2sky@hanmail.net</v>
       </c>
       <c r="E40" t="str">
-        <v xml:space="preserve">Division of Pulmonary Medicine, Department of Medicine, Keio University, School of Medicine, </v>
+        <v xml:space="preserve">Department of Internal Medicine, Seoul National University Hospital, </v>
       </c>
       <c r="F40" t="str">
-        <v>Sato, Toshiro</v>
+        <v>Kim, Tae-You</v>
       </c>
       <c r="G40" t="str">
-        <v>t.sato@keio.jp</v>
+        <v>kimty@snu.ac.kr</v>
       </c>
       <c r="H40" t="str">
-        <v xml:space="preserve">Department of Integrative Medicine and Biochemistry, Keio University School of Medicine, </v>
+        <v xml:space="preserve">Department of Internal Medicine, Seoul National University Hospital, </v>
       </c>
       <c r="L40" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12066730/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6501409/</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Establishment and characterization of an inflammatory cartilaginous organoids model for organoid transplantation study</v>
+        <v>Human Intestinal Morphogenesis Controlled by Transepithelial Morphogen Gradient and Flow-Dependent Physical Cues in a Microengineered Gut-on-a-Chip</v>
       </c>
       <c r="B41" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C41" t="str">
-        <v>Zhang, Yanchao</v>
-      </c>
-      <c r="D41" t="str">
-        <v>docyanchaozhang@163.com</v>
+        <v>Shin, Woojung</v>
       </c>
       <c r="E41" t="str">
-        <v>Department of Orthopedics, China-Japan Friendship Hospital, Beijing, 100029, China</v>
+        <v>Department of Biomedical Engineering, Cockrell School of Engineering, The University of Texas at Austin, Austin, TX 78712, USA</v>
       </c>
       <c r="F41" t="str">
-        <v>Wang, Weiguo</v>
+        <v>Kim, Hyun Jung</v>
       </c>
       <c r="G41" t="str">
-        <v>jointwwg@163.com</v>
+        <v>hyunjung.kim@utexas.edu</v>
       </c>
       <c r="H41" t="str">
-        <v>Department of Orthopedics, China-Japan Friendship Hospital, Beijing, 100029, China</v>
+        <v>Department of Biomedical Engineering, Cockrell School of Engineering, The University of Texas at Austin, Austin, TX 78712, USA</v>
       </c>
       <c r="I41" t="str">
-        <v>Ma, Ruichen</v>
+        <v>Kim, Hyun Jung</v>
       </c>
       <c r="J41" t="str">
-        <v>drmaruichen@163.com</v>
+        <v>hyunjung.kim@utexas.edu</v>
       </c>
       <c r="K41" t="str">
-        <v>Department of Orthopedics, China-Japan Friendship Hospital, Beijing, 100029, China</v>
+        <v>Department of Biomedical Engineering, Cockrell School of Engineering, The University of Texas at Austin, Austin, TX 78712, USA</v>
       </c>
       <c r="L41" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12138948/</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6526295/</v>
+      </c>
+    </row>
+    <row r="42" xml:space="preserve">
       <c r="A42" t="str">
-        <v>Analysis of Biomechanical Characteristics of Bone Tissues Using a Bayesian Neural Network: A Narrative Review</v>
+        <v>Regenerative Medicine of the Bile Duct: Beyond the Myth</v>
       </c>
       <c r="B42" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C42" t="str">
-        <v>Beisekenov, Nail</v>
-      </c>
-      <c r="E42" t="str">
-        <v xml:space="preserve">Graduate School of Science and Technology, Niigata University, Niigata 950-2181, Japan; </v>
+        <v>Buisson, Elina Maria</v>
+      </c>
+      <c r="E42" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Translational Medicine, Graduate School of Biomedical Science and Engineering, Hanyang University, Seoul, 
+</v>
       </c>
       <c r="F42" t="str">
-        <v>Syrnev, Boris</v>
-      </c>
-      <c r="H42" t="str">
-        <v>D. Serikbayev, East Kazakhstan Technical University, 19 Serikbayev Str., Ust-Kamenogorsk 070000, Kazakhstan;  (B.A.);  (B.S.)</v>
-      </c>
-      <c r="I42" t="str">
-        <v>Sadenova, Marzhan</v>
-      </c>
-      <c r="K42" t="str">
-        <v>D. Serikbayev, East Kazakhstan Technical University, 19 Serikbayev Str., Ust-Kamenogorsk 070000, Kazakhstan;  (B.A.);  (B.S.)</v>
+        <v>Choi, Dongho</v>
+      </c>
+      <c r="H42" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Translational Medicine, Graduate School of Biomedical Science and Engineering, Hanyang University, Seoul, 
+</v>
       </c>
       <c r="L42" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12112294/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6657949/</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>A 40-year challenge to resolve clinical questions through experimental/laboratory techniques</v>
+        <v>Epigenetic regulation of mammalian Hedgehog signaling to the stroma determines the molecular subtype of bladder cancer</v>
       </c>
       <c r="B43" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C43" t="str">
-        <v>Iwasaki, Yasumasa</v>
+        <v>Kim, SungEun</v>
       </c>
       <c r="E43" t="str">
-        <v>aff1</v>
+        <v>Calico Life Sciences</v>
       </c>
       <c r="F43" t="str">
-        <v>Iwasaki, Yasumasa</v>
+        <v>Shin, Kunyoo</v>
+      </c>
+      <c r="G43" t="str">
+        <v>kunyoos@postech.ac.kr</v>
       </c>
       <c r="H43" t="str">
-        <v>aff1</v>
+        <v>Calico Life Sciences</v>
       </c>
       <c r="L43" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12086275/</v>
-      </c>
-    </row>
-    <row r="44" xml:space="preserve">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6597241/</v>
+      </c>
+    </row>
+    <row r="44">
       <c r="A44" t="str">
-        <v>Generation and functional characterization of tuft cells in non-human primate pancreatic ducts through organoid culture systems</v>
+        <v>Loss of PKM2 in Lgr5 intestinal stem cells promotes colitis-associated colorectal cancer</v>
       </c>
       <c r="B44" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C44" t="str">
-        <v>Sakaguchi, Kosuke</v>
-      </c>
-      <c r="E44" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Faculty of Applied Bioscience, , , 
-</v>
+        <v>Kim, Yeji</v>
+      </c>
+      <c r="E44" t="str">
+        <v xml:space="preserve">Mucosal Immunology Laboratory, Department of Convergence Medicine, University of Ulsan College of Medicine/Asan Medical Center, </v>
       </c>
       <c r="F44" t="str">
-        <v>Iwatsuki, Ken</v>
-      </c>
-      <c r="H44" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Faculty of Applied Bioscience, , , 
-</v>
-      </c>
-      <c r="I44" t="str">
-        <v>Iwatsuki, Ken</v>
-      </c>
-      <c r="K44" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Faculty of Applied Bioscience, , , 
-</v>
+        <v>Kweon, Mi-Na</v>
+      </c>
+      <c r="G44" t="str">
+        <v>mnkweon@amc.seoul.kr</v>
+      </c>
+      <c r="H44" t="str">
+        <v xml:space="preserve">Mucosal Immunology Laboratory, Department of Convergence Medicine, University of Ulsan College of Medicine/Asan Medical Center, </v>
       </c>
       <c r="L44" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12089129/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6470145/</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>Is Ectopic Cushing Syndrome Commonly Associated with Small Cell Lung Cancer (SCLC)? Critical Review of the Literature and ACTH Expression in Resected SCLC</v>
+        <v>When CAR Meets Stem Cells</v>
       </c>
       <c r="B45" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C45" t="str">
-        <v>Ura, Ayako</v>
+        <v>Lee, Jung Min</v>
       </c>
       <c r="E45" t="str">
-        <v xml:space="preserve">Department of Pathology, Technical University of Munich, TUM School of Medicine and Health, </v>
+        <v/>
       </c>
       <c r="F45" t="str">
-        <v>Kasajima, Atsuko</v>
-      </c>
-      <c r="G45" t="str">
-        <v>atsuko.kasajima@tum.de</v>
+        <v>Lee, Jung Min</v>
       </c>
       <c r="H45" t="str">
-        <v xml:space="preserve">Department of Pathology, Technical University of Munich, TUM School of Medicine and Health, </v>
+        <v/>
       </c>
       <c r="L45" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12048459/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6514932/</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>Comparison of clinicopathologic features and prognosis between surgically resected pulmonary large-cell neuroendocrine carcinoma and small-cell lung cancer</v>
+        <v>A Therapeutic Strategy for Chemotherapy-Resistant Gastric Cancer via Destabilization of Both β-Catenin and RAS</v>
       </c>
       <c r="B46" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C46" t="str">
-        <v>Mao, Yuke</v>
+        <v>Ryu, Won-Ji</v>
       </c>
       <c r="E46" t="str">
-        <v>, , , ;</v>
+        <v>Translational Research Center for Protein Function Control, Yonsei University, Seoul 03722, Korea;  (W.-J.R.);  (Y.-H.C.);  (S.-K.L.);  (J.-H.H.);  (D.S.M.)</v>
       </c>
       <c r="F46" t="str">
-        <v>Wang, Yanan</v>
+        <v>Choi, Kang-Yell</v>
       </c>
       <c r="H46" t="str">
-        <v>, , , ;</v>
+        <v>Translational Research Center for Protein Function Control, Yonsei University, Seoul 03722, Korea;  (W.-J.R.);  (Y.-H.C.);  (S.-K.L.);  (J.-H.H.);  (D.S.M.)</v>
+      </c>
+      <c r="I46" t="str">
+        <v>Cheong, Jae-Ho</v>
+      </c>
+      <c r="K46" t="str">
+        <v>Department of Surgery, Yonsei University College of Medicine, Seoul 03722, Korea;  (J.E.L.);  (S.H.N.)</v>
       </c>
       <c r="L46" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12090107/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6521309/</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>Exploring the Genetic and Clinical Landscape of Dedifferentiated Endometrioid Carcinoma</v>
+        <v>Promotion of Nuclear Medicine-Related Sciences in Developing Countries</v>
       </c>
       <c r="B47" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C47" t="str">
-        <v>Haraga, Hikaru</v>
+        <v>Lee, Dong Soo</v>
+      </c>
+      <c r="D47" t="str">
+        <v>dsl@snu.ac.kr</v>
       </c>
       <c r="E47" t="str">
-        <v>Department of Obstetrics and Gynecology, Faculty of Medicine, Shimane University, 89-1, Enya-Cho, Izumo 693-8501, Shimane, Japan;  (H.H.);  (M.I.);  (H.Y.);  (K.K.)</v>
+        <v xml:space="preserve">Nuclear Medicine, College of Medicine, Seoul National University, </v>
       </c>
       <c r="F47" t="str">
-        <v>Kyo, Satoru</v>
+        <v>Suh, Min Seok</v>
       </c>
       <c r="H47" t="str">
-        <v>Department of Obstetrics and Gynecology, Faculty of Medicine, Shimane University, 89-1, Enya-Cho, Izumo 693-8501, Shimane, Japan;  (H.H.);  (M.I.);  (H.Y.);  (K.K.)</v>
-      </c>
-      <c r="I47" t="str">
-        <v>Nakayama, Kentaro</v>
-      </c>
-      <c r="K47" t="str">
-        <v xml:space="preserve">Department of Obstetrics and Gynecology, Nagoya City University East Medical Center, Nagoya 464-8547, Aichi, Japan; </v>
+        <v xml:space="preserve">Nuclear Medicine, College of Medicine, Seoul National University, </v>
       </c>
       <c r="L47" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12071752/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6473009/</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>Substituents introduction of methyl and methoxy functional groups on resveratrol stabilizes mTOR binding for autophagic cell death induction</v>
+        <v>Large cell neuroendocrine carcinoma arising from uterine endometrium with rapidly progressive course: report of a case and review of literature</v>
       </c>
       <c r="B48" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C48" t="str">
-        <v>Ei, Zin Zin</v>
+        <v>Suh, Dong Soo</v>
       </c>
       <c r="E48" t="str">
-        <v xml:space="preserve">Department of Pharmacology and Physiology, Faculty of Pharmaceutical Sciences, Chulalongkorn university, </v>
+        <v>au1</v>
       </c>
       <c r="F48" t="str">
-        <v>Chanvorachote, Pithi</v>
+        <v>Kim, Ki Hyung</v>
       </c>
       <c r="H48" t="str">
-        <v xml:space="preserve">Department of Pharmacology and Physiology, Faculty of Pharmaceutical Sciences, Chulalongkorn university, </v>
+        <v>au1</v>
       </c>
       <c r="L48" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12033263/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6947078/</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>A tumor-microvessel on-a-chip reveals a mechanism for cancer cell cluster intravasation</v>
+        <v>A subset of diffuse-type gastric cancer is susceptible to mTOR inhibitors and checkpoint inhibitors</v>
       </c>
       <c r="B49" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C49" t="str">
-        <v>Ikeda, Yukinori</v>
+        <v>Fukamachi, Hiroshi</v>
+      </c>
+      <c r="D49" t="str">
+        <v>hfukama.monc@gmail.com</v>
       </c>
       <c r="E49" t="str">
-        <v>Institute of Industrial Science, The University of Tokyo, 4-6-1 Komaba, Meguro-ku, Tokyo 153-8505, Japan</v>
+        <v xml:space="preserve">Department of Molecular Oncology, Graduate School of Medical and Dental Sciences, Tokyo Medical and Dental University, </v>
       </c>
       <c r="F49" t="str">
-        <v>Matsunaga, Yukiko T.</v>
+        <v>Tanaka, Shinji</v>
       </c>
       <c r="G49" t="str">
-        <v>mat@iis.u-tokyo.ac.jp</v>
+        <v>tanaka.monc@tmd.ac.jp</v>
       </c>
       <c r="H49" t="str">
-        <v>Institute of Industrial Science, The University of Tokyo, 4-6-1 Komaba, Meguro-ku, Tokyo 153-8505, Japan</v>
-      </c>
-      <c r="I49" t="str">
-        <v>Oshima, Masanobu</v>
-      </c>
-      <c r="J49" t="str">
-        <v>oshimam@staff.kanazawa-u.ac.jp</v>
-      </c>
-      <c r="K49" t="str">
-        <v>Division of Genetics, Cancer Research Institute, Kanazawa University, Kakuma-machi, Kanazawa 920-1192, Japan</v>
+        <v xml:space="preserve">Department of Molecular Oncology, Graduate School of Medical and Dental Sciences, Tokyo Medical and Dental University, </v>
       </c>
       <c r="L49" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12146038/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6416873/</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>What does “appropriate scientific justification” mean for the review of human pluripotent stem cell, embryo, and related research?</v>
+        <v>Human three-dimensional in vitro model of hepatic zonation to predict zonal hepatotoxicity</v>
       </c>
       <c r="B50" t="str">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="C50" t="str">
-        <v>Jonlin, Erica C.</v>
-      </c>
-      <c r="D50" t="str">
-        <v>ejonlin@uw.edu</v>
+        <v>Ahn, Jaehwan</v>
       </c>
       <c r="E50" t="str">
-        <v>Institute for Stem Cell and Regenerative Medicine, University of Washington, Seattle, WA, USA</v>
+        <v xml:space="preserve">Department of Material Science and Engineering, Korea Advanced Institute of Science and Technology (KAIST), </v>
       </c>
       <c r="F50" t="str">
-        <v>Hyun, Insoo</v>
+        <v>Oh, Jung-Hwa</v>
+      </c>
+      <c r="G50" t="str">
+        <v>jhoh@kitox.re.kr</v>
       </c>
       <c r="H50" t="str">
-        <v>Center for Life Sciences, Museum of Science, Boston, MA, USA</v>
-      </c>
-      <c r="I50" t="str">
-        <v>Jonlin, Erica C.</v>
-      </c>
-      <c r="J50" t="str">
-        <v>ejonlin@uw.edu</v>
-      </c>
-      <c r="K50" t="str">
-        <v>Institute for Stem Cell and Regenerative Medicine, University of Washington, Seattle, WA, USA</v>
+        <v xml:space="preserve">Department of Predictive Toxicology, Korea Institute of Toxicology (KIT), </v>
       </c>
       <c r="L50" t="str">
-        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC12143132/</v>
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6404355/</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Advances in Zika Virus–Host Cell Interaction: Current Knowledge and Future Perspectives</v>
+      </c>
+      <c r="B51" t="str">
+        <v>2019</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Lee, Jae Kyung</v>
+      </c>
+      <c r="E51" t="str">
+        <v/>
+      </c>
+      <c r="F51" t="str">
+        <v>Shin, Ok Sarah</v>
+      </c>
+      <c r="H51" t="str">
+        <v/>
+      </c>
+      <c r="I51" t="str">
+        <v>Shin, Ok Sarah</v>
+      </c>
+      <c r="K51" t="str">
+        <v/>
+      </c>
+      <c r="L51" t="str">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6429326/</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Modeling G2019S-LRRK2 Sporadic Parkinson's Disease in 3D Midbrain Organoids</v>
+      </c>
+      <c r="B52" t="str">
+        <v>2019</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Kim, Hongwon</v>
+      </c>
+      <c r="E52" t="str">
+        <v>Laboratory of Stem Cells &amp; Cell Reprogramming, Department of Biomedical Engineering (BK21Plus Team), Center for Regenerative Medicine, BK21Plus Team for Regenerative Medicine, Dongguk University, Pildong-ro 1-gil 30, Jung-gu, Seoul 04620, Republic of Korea</v>
+      </c>
+      <c r="F52" t="str">
+        <v>Kim, Jongpil</v>
+      </c>
+      <c r="G52" t="str">
+        <v>jpkim153@dongguk.edu</v>
+      </c>
+      <c r="H52" t="str">
+        <v>Laboratory of Stem Cells &amp; Cell Reprogramming, Department of Biomedical Engineering (BK21Plus Team), Center for Regenerative Medicine, BK21Plus Team for Regenerative Medicine, Dongguk University, Pildong-ro 1-gil 30, Jung-gu, Seoul 04620, Republic of Korea</v>
+      </c>
+      <c r="I52" t="str">
+        <v>Kim, Jongpil</v>
+      </c>
+      <c r="J52" t="str">
+        <v>jpkim153@dongguk.edu</v>
+      </c>
+      <c r="K52" t="str">
+        <v>Laboratory of Stem Cells &amp; Cell Reprogramming, Department of Biomedical Engineering (BK21Plus Team), Center for Regenerative Medicine, BK21Plus Team for Regenerative Medicine, Dongguk University, Pildong-ro 1-gil 30, Jung-gu, Seoul 04620, Republic of Korea</v>
+      </c>
+      <c r="L52" t="str">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6410341/</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Resveratrol as a Tumor-Suppressive Nutraceutical Modulating Tumor Microenvironment and Malignant Behaviors of Cancer</v>
+      </c>
+      <c r="B53" t="str">
+        <v>2019</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Han, Youngjin</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Biomodulation, Department of Agricultural Biotechnology, Seoul National University, Seoul 08826, Korea;  (Y.H.);  (H.J.)</v>
+      </c>
+      <c r="F53" t="str">
+        <v>Song, Yong Sang</v>
+      </c>
+      <c r="H53" t="str">
+        <v>Biomodulation, Department of Agricultural Biotechnology, Seoul National University, Seoul 08826, Korea;  (Y.H.);  (H.J.)</v>
+      </c>
+      <c r="I53" t="str">
+        <v>Song, Yong Sang</v>
+      </c>
+      <c r="K53" t="str">
+        <v>Biomodulation, Department of Agricultural Biotechnology, Seoul National University, Seoul 08826, Korea;  (Y.H.);  (H.J.)</v>
+      </c>
+      <c r="L53" t="str">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6412705/</v>
+      </c>
+    </row>
+    <row r="54" xml:space="preserve">
+      <c r="A54" t="str">
+        <v>3D printing approaches for cardiac tissue engineering and role of immune modulation in tissue regeneration</v>
+      </c>
+      <c r="B54" t="str">
+        <v>2019</v>
+      </c>
+      <c r="C54" t="str">
+        <v>Qasim, Muhammad</v>
+      </c>
+      <c r="E54" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Stem Cell and Regenerative Biotechnology, Humanized Pig Research Centre (SRC), Konkuk University, Seoul, South Korea, </v>
+      </c>
+      <c r="F54" t="str">
+        <v>Kim, Jin-Hoi</v>
+      </c>
+      <c r="H54" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Stem Cell and Regenerative Biotechnology, Humanized Pig Research Centre (SRC), Konkuk University, Seoul, South Korea, </v>
+      </c>
+      <c r="I54" t="str">
+        <v>Kim, Jin-Hoi</v>
+      </c>
+      <c r="K54" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Department of Stem Cell and Regenerative Biotechnology, Humanized Pig Research Centre (SRC), Konkuk University, Seoul, South Korea, </v>
+      </c>
+      <c r="L54" t="str">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6388753/</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Analysis of intrahepatic sarcomatoid cholangiocarcinoma: Experience from 11 cases within 17 years</v>
+      </c>
+      <c r="B55" t="str">
+        <v>2019</v>
+      </c>
+      <c r="C55" t="str">
+        <v>Kim, Dong Kyun</v>
+      </c>
+      <c r="E55" t="str">
+        <v/>
+      </c>
+      <c r="F55" t="str">
+        <v>Baek, Yang Hyun</v>
+      </c>
+      <c r="H55" t="str">
+        <v/>
+      </c>
+      <c r="L55" t="str">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6371010/</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Modeling Host-Virus Interactions in Viral Infectious Diseases Using Stem-Cell-Derived Systems and CRISPR/Cas9 Technology</v>
+      </c>
+      <c r="B56" t="str">
+        <v>2019</v>
+      </c>
+      <c r="C56" t="str">
+        <v>Kim, Jihoon</v>
+      </c>
+      <c r="E56" t="str">
+        <v xml:space="preserve">Institute of Molecular Biotechnology of the Austrian Academy of Sciences (IMBA), Vienna Biocenter (VBC), Dr. Bohr-Gasse 3, 1030 Vienna, Austria; </v>
+      </c>
+      <c r="F56" t="str">
+        <v>Yoon, Ki-Jun</v>
+      </c>
+      <c r="H56" t="str">
+        <v>Department of Biological Sciences, Korea Advanced Institute of Science and Technology (KAIST), Daejeon 34141, Korea</v>
+      </c>
+      <c r="I56" t="str">
+        <v>Koo, Bon-Kyoung</v>
+      </c>
+      <c r="K56" t="str">
+        <v xml:space="preserve">Institute of Molecular Biotechnology of the Austrian Academy of Sciences (IMBA), Vienna Biocenter (VBC), Dr. Bohr-Gasse 3, 1030 Vienna, Austria; </v>
+      </c>
+      <c r="L56" t="str">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6409779/</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Organ-on-a-Chip for Cancer and Immune Organs Modeling</v>
+      </c>
+      <c r="B57" t="str">
+        <v>2019</v>
+      </c>
+      <c r="C57" t="str">
+        <v>Sun, Wujin</v>
+      </c>
+      <c r="E57" t="str">
+        <v/>
+      </c>
+      <c r="F57" t="str">
+        <v>Khademhosseini, Ali</v>
+      </c>
+      <c r="H57" t="str">
+        <v/>
+      </c>
+      <c r="L57" t="str">
+        <v>https://pmc.ncbi.nlm.nih.gov/articles/PMC6424124/</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L50"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L57"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>